<commit_message>
ENH: add plots duration time
</commit_message>
<xml_diff>
--- a/data/Base Datos Tercio Medio TESIS.xlsx
+++ b/data/Base Datos Tercio Medio TESIS.xlsx
@@ -1,18 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aranz/Desktop/TESIS DOCTORAL/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB778CA7-83EA-824E-A88D-302C4BFF971D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1665" yWindow="495" windowWidth="29040" windowHeight="16545" activeTab="2"/>
+    <workbookView xWindow="2000" yWindow="900" windowWidth="28800" windowHeight="16540" activeTab="3" xr2:uid="{99F93D72-ECDF-BF45-AD7D-547D28543390}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja 2" sheetId="6" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
     <sheet name="Hoja 4" sheetId="7" r:id="rId4"/>
+    <sheet name="TABLA 1" sheetId="8" r:id="rId5"/>
+    <sheet name="TABLA 2" sheetId="9" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="402">
   <si>
     <t>NHC</t>
   </si>
@@ -936,9 +944,6 @@
     <t>SEXO (V=0, M=1)</t>
   </si>
   <si>
-    <t>LOC (0=Maxilar superior, 1= seno maxilar, 2=nariz-seno etmoidal, 3=órbita, 4=cutáneo)</t>
-  </si>
-  <si>
     <t>AP (0= ca. Epidermoide, 1= Adenocarcinoma, 2= Sarcoma, 3= otros)</t>
   </si>
   <si>
@@ -966,9 +971,6 @@
     <t>RESECCIÓN (BROWN: IIB=0, IID= 1,IIIB=2, IIID=3, IVB=4, IVD=5, V=6, VI=7)</t>
   </si>
   <si>
-    <t>Duración Cirugía</t>
-  </si>
-  <si>
     <t>A.S.M</t>
   </si>
   <si>
@@ -979,13 +981,295 @@
   </si>
   <si>
     <t>si</t>
+  </si>
+  <si>
+    <t>LOC (0=Maxilar superior, 1= seno maxilar, 2=nariz-seno etmoidal, 3=órbita, 4=cutáneo</t>
+  </si>
+  <si>
+    <t>Patient</t>
+  </si>
+  <si>
+    <t>Histology</t>
+  </si>
+  <si>
+    <t>Type of maxillectomy (Brown classification)</t>
+  </si>
+  <si>
+    <t>Stage of disease (AJCC classification)</t>
+  </si>
+  <si>
+    <t>Reconstruction</t>
+  </si>
+  <si>
+    <t>Primary/Recurrence</t>
+  </si>
+  <si>
+    <t>SCC</t>
+  </si>
+  <si>
+    <t>Primary</t>
+  </si>
+  <si>
+    <t>T4a</t>
+  </si>
+  <si>
+    <t>Rectus abdominis</t>
+  </si>
+  <si>
+    <t>Sarcoma</t>
+  </si>
+  <si>
+    <t>OmM</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>Recurrence</t>
+  </si>
+  <si>
+    <t>SOMC flap</t>
+  </si>
+  <si>
+    <t>Temporalis flap</t>
+  </si>
+  <si>
+    <t>Iliac Crest flap</t>
+  </si>
+  <si>
+    <t>Adyuvant Therapy (QT-RT)</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Columna1</t>
+  </si>
+  <si>
+    <t>Am.Ca</t>
+  </si>
+  <si>
+    <t>fibula OMC flap</t>
+  </si>
+  <si>
+    <t>Rectus Abdominis flap</t>
+  </si>
+  <si>
+    <t>Columna2</t>
+  </si>
+  <si>
+    <t>Columna3</t>
+  </si>
+  <si>
+    <t>Columna4</t>
+  </si>
+  <si>
+    <t>Columna5</t>
+  </si>
+  <si>
+    <t>Columna6</t>
+  </si>
+  <si>
+    <t>Columna7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALT </t>
+  </si>
+  <si>
+    <t>690'</t>
+  </si>
+  <si>
+    <t>660'</t>
+  </si>
+  <si>
+    <t>Duración total Cirugía (min)</t>
+  </si>
+  <si>
+    <t>Tiempo ref.</t>
+  </si>
+  <si>
+    <t>Tiempo reg.</t>
+  </si>
+  <si>
+    <t>Tiempo ION</t>
+  </si>
+  <si>
+    <t>4.10</t>
+  </si>
+  <si>
+    <t>4.06</t>
+  </si>
+  <si>
+    <t>3.51</t>
+  </si>
+  <si>
+    <t>3.44</t>
+  </si>
+  <si>
+    <t>3.40</t>
+  </si>
+  <si>
+    <t>3.32</t>
+  </si>
+  <si>
+    <t>3.36</t>
+  </si>
+  <si>
+    <t>3.27</t>
+  </si>
+  <si>
+    <t>3.35</t>
+  </si>
+  <si>
+    <t>3.15</t>
+  </si>
+  <si>
+    <t>3.21</t>
+  </si>
+  <si>
+    <t>3.06</t>
+  </si>
+  <si>
+    <t>2.52</t>
+  </si>
+  <si>
+    <t>2.42</t>
+  </si>
+  <si>
+    <t>3.08</t>
+  </si>
+  <si>
+    <t>3.10</t>
+  </si>
+  <si>
+    <t>2.41</t>
+  </si>
+  <si>
+    <t>2.35</t>
+  </si>
+  <si>
+    <t>2.46</t>
+  </si>
+  <si>
+    <t>2.51</t>
+  </si>
+  <si>
+    <t>5.17</t>
+  </si>
+  <si>
+    <t>5.06</t>
+  </si>
+  <si>
+    <t>5.20</t>
+  </si>
+  <si>
+    <t>4.50</t>
+  </si>
+  <si>
+    <t>4.55</t>
+  </si>
+  <si>
+    <t>4.37</t>
+  </si>
+  <si>
+    <t>4.21</t>
+  </si>
+  <si>
+    <t>4.34</t>
+  </si>
+  <si>
+    <t>4.16</t>
+  </si>
+  <si>
+    <t>4.28</t>
+  </si>
+  <si>
+    <t>4.12</t>
+  </si>
+  <si>
+    <t>3.45</t>
+  </si>
+  <si>
+    <t>3.43</t>
+  </si>
+  <si>
+    <t>3.17</t>
+  </si>
+  <si>
+    <t>3.12</t>
+  </si>
+  <si>
+    <t>3.04</t>
+  </si>
+  <si>
+    <t>2.54</t>
+  </si>
+  <si>
+    <t>12.25</t>
+  </si>
+  <si>
+    <t>10.35</t>
+  </si>
+  <si>
+    <t>11.24</t>
+  </si>
+  <si>
+    <t>9.25</t>
+  </si>
+  <si>
+    <t>9.55</t>
+  </si>
+  <si>
+    <t>10.25</t>
+  </si>
+  <si>
+    <t>9.14</t>
+  </si>
+  <si>
+    <t>8.36</t>
+  </si>
+  <si>
+    <t>7.32</t>
+  </si>
+  <si>
+    <t>8.46</t>
+  </si>
+  <si>
+    <t>10.24</t>
+  </si>
+  <si>
+    <t>11.33</t>
+  </si>
+  <si>
+    <t>8.22</t>
+  </si>
+  <si>
+    <t>6.45</t>
+  </si>
+  <si>
+    <t>7.23</t>
+  </si>
+  <si>
+    <t>8.16</t>
+  </si>
+  <si>
+    <t>9.28</t>
+  </si>
+  <si>
+    <t>7.42</t>
+  </si>
+  <si>
+    <t>6.24</t>
+  </si>
+  <si>
+    <t>6.43</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1155,8 +1439,82 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="18">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Estilo de tabla 1" pivot="0" count="1" xr9:uid="{0BEE9279-42FD-7B43-B8B7-12E9545FB87F}">
+      <tableStyleElement type="wholeTable" dxfId="17"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1166,6 +1524,48 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6BDB3B81-B179-5B40-B258-4808881D0BCF}" name="Tabla1" displayName="Tabla1" ref="A2:G23" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="A2:G23" xr:uid="{6BDB3B81-B179-5B40-B258-4808881D0BCF}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{42483F7B-5CAC-B04A-A2F0-48836FCE4D5B}" name="Columna1" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{63FB591F-23B3-8F47-989A-8D91AF170DFF}" name="Columna2" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{4D804448-FD36-1A43-8145-222CA3C6AE12}" name="Columna3" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{A139671A-0D5C-7D4C-8E37-6F5424CCADA5}" name="Columna4" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{B2E90026-6404-7346-87BF-39601899AF05}" name="Columna5" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{2A623CD3-54F7-1C4D-9F4B-3E50C0D52072}" name="Columna6" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{946D6143-3019-4E41-B22B-9843BB1F1ADF}" name="Columna7" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{32873ABD-2F3C-9943-8EBA-896731903726}" name="Tabla3" displayName="Tabla3" ref="A1:G22" totalsRowShown="0" headerRowDxfId="8" dataDxfId="9">
+  <autoFilter ref="A1:G22" xr:uid="{32873ABD-2F3C-9943-8EBA-896731903726}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{18F0EAFB-6F65-D74C-83BF-B74E09FC0D26}" name="Columna1" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{1AE93DE7-51A2-D44D-98A6-4511AD47D2A7}" name="Columna2" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{46344440-9BCF-A143-A048-65C4FD0D9BEF}" name="Columna3" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{888CE4AD-2E27-4B45-B0B6-092BD2237F89}" name="Columna4" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{C5A132E5-7996-294B-8E92-BC1FDB019133}" name="Columna5" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{194D4E48-17B2-0744-8ED3-12152DBC64EE}" name="Columna6" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{9E3520A3-89C0-0043-8ECF-DA64EA8CD568}" name="Columna7" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2BF61F4D-7C7A-AB46-BC30-ADB54B09998A}" name="Tabla4" displayName="Tabla4" ref="H23:H24" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="H23:H24" xr:uid="{2BF61F4D-7C7A-AB46-BC30-ADB54B09998A}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{BFE76FB1-F749-DC4E-BBC7-E546E97577FE}" name="Columna1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1211,7 +1611,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1263,7 +1663,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1457,41 +1857,41 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C19DE852-6134-424E-9234-BA801BE6A364}">
   <dimension ref="A1:R39"/>
   <sheetViews>
-    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="B21" sqref="A21:XFD21"/>
+    <sheetView topLeftCell="G1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.125" customWidth="1"/>
-    <col min="3" max="3" width="21.375" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
     <col min="4" max="4" width="71.5" customWidth="1"/>
-    <col min="5" max="5" width="31.375" customWidth="1"/>
-    <col min="6" max="6" width="24.125" customWidth="1"/>
-    <col min="7" max="7" width="40.125" customWidth="1"/>
+    <col min="5" max="5" width="31.33203125" customWidth="1"/>
+    <col min="6" max="6" width="24.1640625" customWidth="1"/>
+    <col min="7" max="7" width="40.1640625" customWidth="1"/>
     <col min="8" max="8" width="44" customWidth="1"/>
-    <col min="9" max="9" width="20.125" customWidth="1"/>
-    <col min="10" max="10" width="32.125" customWidth="1"/>
-    <col min="11" max="11" width="32.625" customWidth="1"/>
-    <col min="13" max="13" width="33.625" customWidth="1"/>
-    <col min="14" max="14" width="35.625" customWidth="1"/>
-    <col min="15" max="15" width="64.125" customWidth="1"/>
+    <col min="9" max="9" width="20.1640625" customWidth="1"/>
+    <col min="10" max="10" width="32.1640625" customWidth="1"/>
+    <col min="11" max="11" width="32.6640625" customWidth="1"/>
+    <col min="13" max="13" width="33.6640625" customWidth="1"/>
+    <col min="14" max="14" width="35.6640625" customWidth="1"/>
+    <col min="15" max="15" width="64.1640625" customWidth="1"/>
     <col min="16" max="16" width="44" customWidth="1"/>
-    <col min="17" max="17" width="14.375" customWidth="1"/>
-    <col min="18" max="18" width="54.875" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" customWidth="1"/>
+    <col min="18" max="18" width="54.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>240</v>
       </c>
@@ -1547,7 +1947,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
@@ -1601,7 +2001,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
@@ -1655,7 +2055,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>8</v>
       </c>
@@ -1709,7 +2109,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>9</v>
       </c>
@@ -1763,7 +2163,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
@@ -1815,7 +2215,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>11</v>
       </c>
@@ -1871,7 +2271,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>12</v>
       </c>
@@ -1923,7 +2323,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>41</v>
       </c>
@@ -1975,7 +2375,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>50</v>
       </c>
@@ -2025,7 +2425,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>54</v>
       </c>
@@ -2075,9 +2475,9 @@
         <v>164</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B12" s="8">
         <v>525800</v>
@@ -2125,7 +2525,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>61</v>
       </c>
@@ -2177,7 +2577,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>95</v>
       </c>
@@ -2231,7 +2631,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>113</v>
       </c>
@@ -2281,7 +2681,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>127</v>
       </c>
@@ -2335,7 +2735,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>131</v>
       </c>
@@ -2383,7 +2783,7 @@
       <c r="Q17" s="7"/>
       <c r="R17" s="7"/>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>216</v>
       </c>
@@ -2439,7 +2839,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>224</v>
       </c>
@@ -2487,7 +2887,7 @@
       <c r="Q19" s="7"/>
       <c r="R19" s="7"/>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>229</v>
       </c>
@@ -2537,7 +2937,7 @@
       <c r="Q20" s="7"/>
       <c r="R20" s="7"/>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>262</v>
       </c>
@@ -2584,10 +2984,10 @@
         <v>267</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -2607,7 +3007,7 @@
       <c r="Q23" s="2"/>
       <c r="R23" s="3"/>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -2626,7 +3026,7 @@
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -2642,7 +3042,7 @@
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -2658,7 +3058,7 @@
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2672,7 +3072,7 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -2689,7 +3089,7 @@
       <c r="N28" s="7"/>
       <c r="O28" s="1"/>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2704,7 +3104,7 @@
       <c r="M29" s="1"/>
       <c r="O29" s="1"/>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -2720,7 +3120,7 @@
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -2736,7 +3136,7 @@
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -2752,7 +3152,7 @@
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -2768,7 +3168,7 @@
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -2784,7 +3184,7 @@
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -2799,7 +3199,7 @@
       <c r="L35" s="8"/>
       <c r="M35" s="8"/>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -2815,7 +3215,7 @@
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -2830,7 +3230,7 @@
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -2846,7 +3246,7 @@
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -2871,31 +3271,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B9EA37-FED7-7046-A8CF-EB7B08CDC7AF}">
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.875" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="3" max="3" width="25.5" customWidth="1"/>
-    <col min="4" max="4" width="48.875" customWidth="1"/>
-    <col min="6" max="6" width="25.625" customWidth="1"/>
-    <col min="7" max="7" width="35.625" customWidth="1"/>
+    <col min="4" max="4" width="48.83203125" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" customWidth="1"/>
+    <col min="7" max="7" width="35.6640625" customWidth="1"/>
     <col min="8" max="8" width="43.5" customWidth="1"/>
-    <col min="9" max="9" width="14.875" customWidth="1"/>
-    <col min="11" max="11" width="32.375" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" customWidth="1"/>
+    <col min="11" max="11" width="32.33203125" customWidth="1"/>
     <col min="13" max="13" width="17.5" customWidth="1"/>
     <col min="14" max="14" width="44.5" customWidth="1"/>
-    <col min="15" max="15" width="45.875" customWidth="1"/>
+    <col min="15" max="15" width="45.83203125" customWidth="1"/>
     <col min="16" max="16" width="25" customWidth="1"/>
-    <col min="18" max="18" width="40.875" customWidth="1"/>
+    <col min="18" max="18" width="40.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="6"/>
       <c r="B1" s="10" t="s">
         <v>0</v>
@@ -2949,12 +3349,12 @@
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>231</v>
       </c>
@@ -3011,7 +3411,7 @@
       <c r="T3" s="7"/>
       <c r="U3" s="7"/>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>235</v>
       </c>
@@ -3064,7 +3464,7 @@
       <c r="T4" s="7"/>
       <c r="U4" s="7"/>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>64</v>
       </c>
@@ -3115,7 +3515,7 @@
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>66</v>
       </c>
@@ -3166,7 +3566,7 @@
       <c r="T6" s="7"/>
       <c r="U6" s="7"/>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>68</v>
       </c>
@@ -3215,7 +3615,7 @@
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>69</v>
       </c>
@@ -3266,7 +3666,7 @@
       <c r="T8" s="7"/>
       <c r="U8" s="7"/>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>73</v>
       </c>
@@ -3315,7 +3715,7 @@
       <c r="T9" s="7"/>
       <c r="U9" s="7"/>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>74</v>
       </c>
@@ -3366,7 +3766,7 @@
       <c r="T10" s="7"/>
       <c r="U10" s="7"/>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>76</v>
       </c>
@@ -3419,7 +3819,7 @@
       <c r="T11" s="7"/>
       <c r="U11" s="7"/>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>83</v>
       </c>
@@ -3470,7 +3870,7 @@
       <c r="T12" s="7"/>
       <c r="U12" s="7"/>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>88</v>
       </c>
@@ -3523,7 +3923,7 @@
       <c r="T13" s="7"/>
       <c r="U13" s="7"/>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>89</v>
       </c>
@@ -3574,7 +3974,7 @@
       <c r="T14" s="7"/>
       <c r="U14" s="7"/>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>91</v>
       </c>
@@ -3623,7 +4023,7 @@
       <c r="T15" s="7"/>
       <c r="U15" s="7"/>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>235</v>
       </c>
@@ -3674,7 +4074,7 @@
       <c r="T16" s="7"/>
       <c r="U16" s="7"/>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>112</v>
       </c>
@@ -3723,7 +4123,7 @@
       <c r="T17" s="7"/>
       <c r="U17" s="7"/>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>115</v>
       </c>
@@ -3774,7 +4174,7 @@
       <c r="T18" s="7"/>
       <c r="U18" s="7"/>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>241</v>
       </c>
@@ -3825,7 +4225,7 @@
       <c r="T19" s="7"/>
       <c r="U19" s="7"/>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>245</v>
       </c>
@@ -3876,7 +4276,7 @@
       <c r="T20" s="7"/>
       <c r="U20" s="7"/>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>249</v>
       </c>
@@ -3920,9 +4320,9 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B22" s="8">
         <v>250522</v>
@@ -3934,13 +4334,13 @@
         <v>108</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G22" s="17">
         <v>0</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J22" s="23">
         <v>37966</v>
@@ -3955,10 +4355,10 @@
         <v>1</v>
       </c>
       <c r="P22" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="Q22" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -3967,27 +4367,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23E6AEDD-AB0E-E144-ADD1-080FF1FDCD6F}">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView topLeftCell="A8" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.625" customWidth="1"/>
-    <col min="5" max="5" width="16.375" customWidth="1"/>
-    <col min="6" max="6" width="13.625" customWidth="1"/>
-    <col min="7" max="7" width="12.125" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>174</v>
       </c>
@@ -4019,7 +4419,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>181</v>
       </c>
@@ -4051,7 +4451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>182</v>
       </c>
@@ -4083,7 +4483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>183</v>
       </c>
@@ -4115,7 +4515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>184</v>
       </c>
@@ -4147,7 +4547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>185</v>
       </c>
@@ -4179,7 +4579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>186</v>
       </c>
@@ -4211,7 +4611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>187</v>
       </c>
@@ -4243,7 +4643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>188</v>
       </c>
@@ -4275,7 +4675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>268</v>
       </c>
@@ -4307,7 +4707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>189</v>
       </c>
@@ -4339,7 +4739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>190</v>
       </c>
@@ -4371,7 +4771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>191</v>
       </c>
@@ -4403,7 +4803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>192</v>
       </c>
@@ -4435,7 +4835,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>193</v>
       </c>
@@ -4468,7 +4868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>194</v>
       </c>
@@ -4500,7 +4900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>195</v>
       </c>
@@ -4532,7 +4932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>269</v>
       </c>
@@ -4564,7 +4964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>270</v>
       </c>
@@ -4596,7 +4996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>271</v>
       </c>
@@ -4628,7 +5028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>272</v>
       </c>
@@ -4660,7 +5060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I23" s="18">
         <f>SUM(I3:I22)</f>
         <v>105</v>
@@ -4676,7 +5076,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>274</v>
       </c>
@@ -4693,12 +5093,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
         <v>40</v>
       </c>
@@ -4721,7 +5121,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>280</v>
       </c>
@@ -4753,7 +5153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>543490</v>
       </c>
@@ -4785,7 +5185,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>198</v>
       </c>
@@ -4817,7 +5217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>199</v>
       </c>
@@ -4849,7 +5249,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>200</v>
       </c>
@@ -4881,7 +5281,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>201</v>
       </c>
@@ -4913,7 +5313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>202</v>
       </c>
@@ -4945,7 +5345,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>203</v>
       </c>
@@ -4977,7 +5377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>204</v>
       </c>
@@ -5009,7 +5409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>205</v>
       </c>
@@ -5041,7 +5441,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>206</v>
       </c>
@@ -5073,7 +5473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>207</v>
       </c>
@@ -5105,7 +5505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>281</v>
       </c>
@@ -5137,7 +5537,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
         <v>208</v>
       </c>
@@ -5169,7 +5569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
         <v>209</v>
       </c>
@@ -5201,7 +5601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>210</v>
       </c>
@@ -5233,7 +5633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
         <v>211</v>
       </c>
@@ -5265,7 +5665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>282</v>
       </c>
@@ -5297,7 +5697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>283</v>
       </c>
@@ -5329,7 +5729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>284</v>
       </c>
@@ -5361,7 +5761,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I48" s="18">
         <v>91</v>
       </c>
@@ -5375,7 +5775,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
         <v>214</v>
       </c>
@@ -5392,7 +5792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
         <v>215</v>
       </c>
@@ -5403,40 +5803,40 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15FA894E-06A8-4645-BB3F-F1560FD668EC}">
+  <dimension ref="A1:AA41"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="W34" sqref="W34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="5" max="5" width="16.375" customWidth="1"/>
-    <col min="6" max="6" width="13.625" customWidth="1"/>
-    <col min="7" max="7" width="12.125" customWidth="1"/>
-    <col min="12" max="12" width="20.375" customWidth="1"/>
-    <col min="13" max="13" width="37.625" customWidth="1"/>
-    <col min="14" max="14" width="32.125" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" customWidth="1"/>
+    <col min="13" max="13" width="37.6640625" customWidth="1"/>
+    <col min="14" max="14" width="32.1640625" customWidth="1"/>
     <col min="15" max="15" width="22" customWidth="1"/>
-    <col min="16" max="16" width="18.625" customWidth="1"/>
-    <col min="17" max="17" width="20.875" customWidth="1"/>
-    <col min="18" max="18" width="16.375" customWidth="1"/>
+    <col min="16" max="16" width="18.6640625" customWidth="1"/>
+    <col min="17" max="17" width="20.83203125" customWidth="1"/>
+    <col min="18" max="18" width="16.33203125" customWidth="1"/>
     <col min="19" max="19" width="13" customWidth="1"/>
-    <col min="20" max="20" width="18" customWidth="1"/>
-    <col min="21" max="21" width="26.375" customWidth="1"/>
-    <col min="22" max="22" width="15.375" customWidth="1"/>
-    <col min="23" max="23" width="31.375" customWidth="1"/>
-    <col min="24" max="24" width="17.375" customWidth="1"/>
+    <col min="20" max="20" width="21.1640625" customWidth="1"/>
+    <col min="21" max="21" width="26.33203125" customWidth="1"/>
+    <col min="22" max="22" width="27" customWidth="1"/>
+    <col min="23" max="23" width="31.33203125" customWidth="1"/>
+    <col min="24" max="24" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>288</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>176</v>
@@ -5469,43 +5869,52 @@
         <v>294</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>300</v>
-      </c>
       <c r="T1" s="1" t="s">
-        <v>305</v>
+        <v>341</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -5563,8 +5972,20 @@
       <c r="S2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:24">
+      <c r="T2" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -5622,8 +6043,20 @@
       <c r="S3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:24">
+      <c r="T3" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -5681,8 +6114,20 @@
       <c r="S4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:24">
+      <c r="T4" s="1">
+        <v>330</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -5740,8 +6185,20 @@
       <c r="S5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:24">
+      <c r="T5" s="1">
+        <v>705</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -5799,8 +6256,20 @@
       <c r="S6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:24">
+      <c r="T6" s="1">
+        <v>545</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -5858,8 +6327,20 @@
       <c r="S7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:24">
+      <c r="T7" s="1">
+        <v>657</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -5917,8 +6398,20 @@
       <c r="S8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:24">
+      <c r="T8" s="1">
+        <v>517</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -5976,8 +6469,20 @@
       <c r="S9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:24">
+      <c r="T9" s="1">
+        <v>738</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -6035,8 +6540,20 @@
       <c r="S10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:24">
+      <c r="T10" s="1">
+        <v>606</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -6094,8 +6611,20 @@
       <c r="S11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:24">
+      <c r="T11" s="1">
+        <v>312</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -6153,8 +6682,20 @@
       <c r="S12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:24">
+      <c r="T12" s="1">
+        <v>614</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -6212,8 +6753,20 @@
       <c r="S13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:24">
+      <c r="T13" s="1">
+        <v>674</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -6271,8 +6824,20 @@
       <c r="S14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:24">
+      <c r="T14" s="1">
+        <v>316</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -6330,8 +6895,20 @@
       <c r="S15" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:24">
+      <c r="T15" s="1">
+        <v>569</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -6389,8 +6966,20 @@
       <c r="S16" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:19">
+      <c r="T16" s="1">
+        <v>713</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -6448,8 +7037,20 @@
       <c r="S17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:19">
+      <c r="T17" s="1">
+        <v>532</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -6507,8 +7108,20 @@
       <c r="S18" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:19">
+      <c r="T18" s="1">
+        <v>483</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -6566,8 +7179,20 @@
       <c r="S19" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:19">
+      <c r="T19" s="1">
+        <v>686</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -6625,8 +7250,20 @@
       <c r="S20" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:19">
+      <c r="T20" s="1">
+        <v>622</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="W20" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -6684,8 +7321,20 @@
       <c r="S21" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:19">
+      <c r="T21" s="1">
+        <v>618</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>0</v>
       </c>
@@ -6723,7 +7372,7 @@
         <v>0</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="N22" s="1">
         <v>0</v>
@@ -6743,8 +7392,11 @@
       <c r="S22" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:19">
+      <c r="T22" s="1">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>0</v>
       </c>
@@ -6802,8 +7454,11 @@
       <c r="S23" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:19">
+      <c r="T23" s="1">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>0</v>
       </c>
@@ -6841,7 +7496,7 @@
         <v>0</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="N24" s="1">
         <v>0</v>
@@ -6861,8 +7516,11 @@
       <c r="S24" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:19">
+      <c r="T24" s="1">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>0</v>
       </c>
@@ -6920,8 +7578,11 @@
       <c r="S25" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:19">
+      <c r="T25" s="1">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>0</v>
       </c>
@@ -6959,7 +7620,7 @@
         <v>1</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="N26" s="1">
         <v>0</v>
@@ -6979,8 +7640,11 @@
       <c r="S26" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:19">
+      <c r="T26" s="1">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>0</v>
       </c>
@@ -7038,8 +7702,11 @@
       <c r="S27" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:19">
+      <c r="T27" s="1">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>0</v>
       </c>
@@ -7097,8 +7764,11 @@
       <c r="S28" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:19">
+      <c r="T28" s="1">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>0</v>
       </c>
@@ -7156,8 +7826,11 @@
       <c r="S29" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:19">
+      <c r="T29" s="1">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>0</v>
       </c>
@@ -7215,8 +7888,11 @@
       <c r="S30" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:19">
+      <c r="T30" s="1">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>0</v>
       </c>
@@ -7274,8 +7950,11 @@
       <c r="S31" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:19">
+      <c r="T31" s="1">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>0</v>
       </c>
@@ -7333,8 +8012,11 @@
       <c r="S32" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:19">
+      <c r="T32" s="1">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>0</v>
       </c>
@@ -7392,8 +8074,11 @@
       <c r="S33" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:19">
+      <c r="T33" s="1">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>0</v>
       </c>
@@ -7451,8 +8136,11 @@
       <c r="S34" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:19">
+      <c r="T34" s="1">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>0</v>
       </c>
@@ -7510,8 +8198,11 @@
       <c r="S35" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:19">
+      <c r="T35" s="1">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>0</v>
       </c>
@@ -7569,8 +8260,11 @@
       <c r="S36" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:19">
+      <c r="T36" s="1">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>0</v>
       </c>
@@ -7628,8 +8322,11 @@
       <c r="S37" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:19">
+      <c r="T37" s="1">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>0</v>
       </c>
@@ -7687,8 +8384,11 @@
       <c r="S38" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:19">
+      <c r="T38" s="1">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>0</v>
       </c>
@@ -7746,8 +8446,11 @@
       <c r="S39" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:19">
+      <c r="T39" s="1">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>0</v>
       </c>
@@ -7805,8 +8508,11 @@
       <c r="S40" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:19">
+      <c r="T40" s="1">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>0</v>
       </c>
@@ -7863,9 +8569,1084 @@
       </c>
       <c r="S41" s="1">
         <v>1</v>
+      </c>
+      <c r="T41" s="1">
+        <v>812</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E24E263D-5633-1941-9C86-B09365C24072}">
+  <dimension ref="A2:G23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.5" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C2" t="s">
+        <v>333</v>
+      </c>
+      <c r="D2" t="s">
+        <v>334</v>
+      </c>
+      <c r="E2" t="s">
+        <v>335</v>
+      </c>
+      <c r="F2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>15</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>19</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A777D94-5111-FC49-ABC4-F691260C39A5}">
+  <dimension ref="A1:H23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>336</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H23" t="s">
+        <v>328</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>